<commit_message>
request template rows dynamic added, layout beta implemented, select component updated
</commit_message>
<xml_diff>
--- a/templates/Request_Contract_Ru.xlsx
+++ b/templates/Request_Contract_Ru.xlsx
@@ -8,27 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{977C10C7-FA9F-43E4-9952-2C6F3BC8E755}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97F68409-F5FB-4A51-B257-2302FE16DCBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{D30FD3A5-3631-4292-86EF-527B77EA97BF}"/>
+    <workbookView xWindow="-55778" yWindow="-907" windowWidth="28995" windowHeight="15795" xr2:uid="{D30FD3A5-3631-4292-86EF-527B77EA97BF}"/>
   </bookViews>
   <sheets>
-    <sheet name="Заявки на договора" sheetId="1" r:id="rId1"/>
+    <sheet name="Request_Contract" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Заявки на договора'!$A$1:$G$48</definedName>
-    <definedName name="Банковские_реквизиты">'Заявки на договора'!$A$30</definedName>
-    <definedName name="ВСД">'Заявки на договора'!$A$36</definedName>
-    <definedName name="ВСД_далее">'Заявки на договора'!$A$37</definedName>
-    <definedName name="Доставка_условия">'Заявки на договора'!$A$23</definedName>
-    <definedName name="Заявка">'Заявки на договора'!$A$4</definedName>
-    <definedName name="Заявка_дата">'Заявки на договора'!$G$3</definedName>
-    <definedName name="Заявка_массив">'Заявки на договора'!$A$9</definedName>
-    <definedName name="Заявка_стороны">'Заявки на договора'!$A$6</definedName>
-    <definedName name="Оплата_дата">'Заявки на договора'!$A$24</definedName>
-    <definedName name="Прибытие">'Заявки на договора'!$A$32</definedName>
-    <definedName name="Приемка">'Заявки на договора'!$A$34</definedName>
-    <definedName name="Сумма">'Заявки на договора'!$A$22</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Request_Contract!$A$1:$G$45</definedName>
+    <definedName name="Банковские_реквизиты">Request_Contract!$A$19</definedName>
+    <definedName name="ВСД">Request_Contract!$A$25</definedName>
+    <definedName name="ВСД_далее">Request_Contract!$A$26</definedName>
+    <definedName name="Доставка_условия">Request_Contract!$A$12</definedName>
+    <definedName name="Заявка">Request_Contract!$A$4</definedName>
+    <definedName name="Заявка_дата">Request_Contract!$G$3</definedName>
+    <definedName name="Заявка_массив">Request_Contract!$A$9</definedName>
+    <definedName name="Заявка_стороны">Request_Contract!$A$6</definedName>
+    <definedName name="Оплата_дата">Request_Contract!$A$13</definedName>
+    <definedName name="Прибытие">Request_Contract!$A$21</definedName>
+    <definedName name="Приемка">Request_Contract!$A$23</definedName>
+    <definedName name="Сумма">Request_Contract!$A$11</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t>З А Я В К А</t>
   </si>
@@ -71,12 +71,6 @@
     <t>Упаковка</t>
   </si>
   <si>
-    <t>Кол-во</t>
-  </si>
-  <si>
-    <t>Цена</t>
-  </si>
-  <si>
     <t xml:space="preserve">Сумма, руб. </t>
   </si>
   <si>
@@ -122,9 +116,6 @@
     <t>25+</t>
   </si>
   <si>
-    <t>27+</t>
-  </si>
-  <si>
     <t>Сумма по договору : 14 745 588,00 ₽</t>
   </si>
   <si>
@@ -159,16 +150,21 @@
   </si>
   <si>
     <t>Прошу разработать договор поставки № 569 от 10.04.2023 г.</t>
+  </si>
+  <si>
+    <t>Кол-во, кг</t>
+  </si>
+  <si>
+    <t>Цена, руб</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="&quot;1/&quot;#,##0.0&quot; кг&quot;"/>
-    <numFmt numFmtId="165" formatCode="#,##0.0"/>
-    <numFmt numFmtId="166" formatCode="#,##0.00&quot;₽&quot;"/>
+    <numFmt numFmtId="172" formatCode="#,##0.00\ &quot;₽&quot;"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -264,7 +260,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -279,9 +275,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -297,35 +290,43 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="172" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -375,7 +376,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>1003301</xdr:colOff>
+      <xdr:colOff>1003300</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>7771</xdr:rowOff>
     </xdr:to>
@@ -723,167 +724,167 @@
     <tabColor theme="5" tint="0.39997558519241921"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:V48"/>
+  <dimension ref="A1:V45"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="76" zoomScaleNormal="100" zoomScaleSheetLayoutView="76" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="84" zoomScaleNormal="100" zoomScaleSheetLayoutView="84" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="24.3984375" style="7" customWidth="1"/>
-    <col min="2" max="2" width="21.46484375" style="7" customWidth="1"/>
-    <col min="3" max="3" width="9.73046875" style="7" customWidth="1"/>
-    <col min="4" max="4" width="33.73046875" style="7" customWidth="1"/>
-    <col min="5" max="5" width="15.19921875" style="7" customWidth="1"/>
-    <col min="6" max="6" width="12.73046875" style="7" customWidth="1"/>
-    <col min="7" max="7" width="15.59765625" style="7" customWidth="1"/>
-    <col min="8" max="8" width="14.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.796875" style="7"/>
-    <col min="10" max="10" width="22.33203125" style="7" customWidth="1"/>
-    <col min="11" max="11" width="17" style="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.796875" style="7" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="0" style="7" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="6.796875" style="7" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="10" style="7" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="8" style="7" hidden="1" customWidth="1"/>
-    <col min="17" max="18" width="0" style="7" hidden="1" customWidth="1"/>
-    <col min="19" max="20" width="8.796875" style="7" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="14.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="8.796875" style="7"/>
+    <col min="1" max="1" width="24.3984375" style="6" customWidth="1"/>
+    <col min="2" max="2" width="21.46484375" style="6" customWidth="1"/>
+    <col min="3" max="3" width="7.1328125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="37.6640625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="12.73046875" style="18" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" style="23" customWidth="1"/>
+    <col min="7" max="7" width="15.59765625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.796875" style="6"/>
+    <col min="10" max="10" width="22.33203125" style="6" customWidth="1"/>
+    <col min="11" max="11" width="17" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.796875" style="6" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="0" style="6" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="6.796875" style="6" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="10" style="6" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="8" style="6" hidden="1" customWidth="1"/>
+    <col min="17" max="18" width="0" style="6" hidden="1" customWidth="1"/>
+    <col min="19" max="20" width="8.796875" style="6" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="14.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="8.796875" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="30.75" x14ac:dyDescent="0.5">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="22"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="13"/>
       <c r="I1"/>
       <c r="J1"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="8"/>
-      <c r="S1" s="8"/>
-      <c r="T1" s="8"/>
-      <c r="U1" s="8"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.5">
-      <c r="A2" s="9"/>
+      <c r="A2" s="8"/>
       <c r="I2"/>
       <c r="J2"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
-      <c r="P2" s="8"/>
-      <c r="Q2" s="8"/>
-      <c r="R2" s="8"/>
-      <c r="S2" s="8"/>
-      <c r="T2" s="8"/>
-      <c r="U2" s="8"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="7"/>
+      <c r="U2" s="7"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.5">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="10">
+      <c r="G3" s="9">
         <v>45026</v>
       </c>
       <c r="I3"/>
       <c r="J3"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="8"/>
-      <c r="U3" s="8"/>
-      <c r="V3" s="11"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
+      <c r="U3" s="7"/>
+      <c r="V3" s="10"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.5">
       <c r="A4" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="I4"/>
       <c r="J4"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="8"/>
-      <c r="O4" s="8"/>
-      <c r="P4" s="8"/>
-      <c r="Q4" s="8"/>
-      <c r="R4" s="8"/>
-      <c r="S4" s="8"/>
-      <c r="T4" s="8"/>
-      <c r="U4" s="8"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="7"/>
+      <c r="U4" s="7"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.5">
       <c r="A5" s="2"/>
       <c r="I5"/>
       <c r="J5"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="8"/>
-      <c r="P5" s="8"/>
-      <c r="Q5" s="8"/>
-      <c r="R5" s="8"/>
-      <c r="S5" s="8"/>
-      <c r="T5" s="8"/>
-      <c r="U5" s="8"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="7"/>
+      <c r="S5" s="7"/>
+      <c r="T5" s="7"/>
+      <c r="U5" s="7"/>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.5">
       <c r="A6" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="I6"/>
       <c r="J6"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="8"/>
-      <c r="O6" s="8"/>
-      <c r="P6" s="8"/>
-      <c r="Q6" s="8"/>
-      <c r="R6" s="8"/>
-      <c r="S6" s="8"/>
-      <c r="T6" s="8"/>
-      <c r="U6" s="8"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="7"/>
+      <c r="S6" s="7"/>
+      <c r="T6" s="7"/>
+      <c r="U6" s="7"/>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.5">
       <c r="A7" s="2"/>
       <c r="I7"/>
       <c r="J7"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="8"/>
-      <c r="P7" s="8"/>
-      <c r="Q7" s="8"/>
-      <c r="R7" s="8"/>
-      <c r="S7" s="8"/>
-      <c r="T7" s="8"/>
-      <c r="U7" s="8"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="7"/>
+      <c r="S7" s="7"/>
+      <c r="T7" s="7"/>
+      <c r="U7" s="7"/>
     </row>
     <row r="8" spans="1:22" ht="39" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A8" s="3" t="s">
@@ -898,207 +899,195 @@
       <c r="D8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8" s="25" t="s">
         <v>6</v>
-      </c>
-      <c r="F8" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>8</v>
       </c>
       <c r="H8"/>
       <c r="I8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="8"/>
-      <c r="Q8" s="8"/>
-      <c r="R8" s="8"/>
-      <c r="S8" s="8"/>
-      <c r="T8" s="8"/>
-    </row>
-    <row r="9" spans="1:22" ht="76.5" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="7"/>
+      <c r="S8" s="7"/>
+      <c r="T8" s="7"/>
+    </row>
+    <row r="9" spans="1:22" ht="68.650000000000006" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" s="14">
+      <c r="D9" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="20">
         <v>172939</v>
       </c>
-      <c r="F9" s="15">
+      <c r="F9" s="16">
         <v>36</v>
       </c>
-      <c r="G9" s="16">
+      <c r="G9" s="26">
         <v>6225804</v>
       </c>
       <c r="H9"/>
       <c r="I9"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8"/>
-      <c r="P9" s="8"/>
-      <c r="Q9" s="8"/>
-      <c r="R9" s="8"/>
-      <c r="S9" s="8"/>
-      <c r="T9" s="8"/>
-    </row>
-    <row r="10" spans="1:22" ht="76.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A10" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="4" t="s">
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="7"/>
+      <c r="S9" s="7"/>
+      <c r="T9" s="7"/>
+    </row>
+    <row r="10" spans="1:22" ht="79.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="G10" s="23"/>
+      <c r="I10"/>
+      <c r="J10"/>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.5">
+      <c r="A11" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="14">
-        <v>205296</v>
-      </c>
-      <c r="F10" s="15">
-        <v>41.5</v>
-      </c>
-      <c r="G10" s="16">
-        <v>8519784</v>
-      </c>
-      <c r="H10"/>
-      <c r="I10"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="8"/>
-      <c r="O10" s="8"/>
-      <c r="P10" s="8"/>
-      <c r="Q10" s="8"/>
-      <c r="R10" s="8"/>
-      <c r="S10" s="8"/>
-      <c r="T10" s="8"/>
-    </row>
-    <row r="11" spans="1:22" ht="39.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A11" s="4"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="16"/>
+      <c r="G11" s="23"/>
       <c r="I11"/>
       <c r="J11"/>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.5">
-      <c r="A12" s="4"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="20"/>
+      <c r="A12" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" s="23"/>
       <c r="I12"/>
       <c r="J12"/>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.5">
+      <c r="A13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="23"/>
       <c r="I13"/>
       <c r="J13"/>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.5">
+      <c r="A14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G14" s="23"/>
       <c r="I14"/>
       <c r="J14"/>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.5">
+      <c r="A15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G15" s="23"/>
       <c r="I15"/>
       <c r="J15"/>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:22" ht="30.4" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16" s="23"/>
       <c r="I16"/>
       <c r="J16"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A17" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G17" s="23"/>
       <c r="I17"/>
       <c r="J17"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A18" s="2"/>
+      <c r="G18" s="23"/>
       <c r="I18"/>
       <c r="J18"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G19" s="23"/>
       <c r="I19"/>
       <c r="J19"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A20" s="2"/>
+      <c r="G20" s="23"/>
       <c r="I20"/>
       <c r="J20"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A21" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G21" s="23"/>
       <c r="I21"/>
       <c r="J21"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A22" s="6" t="s">
-        <v>24</v>
-      </c>
+      <c r="A22" s="2"/>
+      <c r="G22" s="23"/>
       <c r="I22"/>
       <c r="J22"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="2" t="s">
         <v>25</v>
       </c>
       <c r="I23"/>
       <c r="J23"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A24" s="2" t="s">
-        <v>26</v>
-      </c>
+      <c r="A24" s="2"/>
       <c r="I24"/>
       <c r="J24"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A25" s="2" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="I25"/>
       <c r="J25"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A26" s="2" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="I26"/>
       <c r="J26"/>
     </row>
-    <row r="27" spans="1:10" ht="30.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A27" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I27"/>
       <c r="J27"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A28" s="5" t="s">
-        <v>33</v>
-      </c>
+      <c r="A28" s="2"/>
       <c r="I28"/>
       <c r="J28"/>
     </row>
@@ -1108,20 +1097,20 @@
       <c r="J29"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A30" s="2" t="s">
-        <v>27</v>
-      </c>
+      <c r="A30" s="2"/>
       <c r="I30"/>
       <c r="J30"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A31" s="2"/>
+      <c r="A31" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="I31"/>
       <c r="J31"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A32" s="2" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="I32"/>
       <c r="J32"/>
@@ -1133,122 +1122,63 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A34" s="2" t="s">
-        <v>28</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
       <c r="I34"/>
       <c r="J34"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A35" s="2"/>
+      <c r="A35" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="I35"/>
       <c r="J35"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A36" s="2" t="s">
-        <v>29</v>
-      </c>
+      <c r="A36" s="2"/>
       <c r="I36"/>
       <c r="J36"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A37" s="2" t="s">
-        <v>30</v>
+        <v>16</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="21" t="s">
+        <v>14</v>
       </c>
       <c r="I37"/>
       <c r="J37"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A38" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I38"/>
-      <c r="J38"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A39" s="2"/>
-      <c r="I39"/>
-      <c r="J39"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A40" s="2"/>
-      <c r="I40"/>
-      <c r="J40"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A41" s="2"/>
-      <c r="I41"/>
-      <c r="J41"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A42" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I42"/>
-      <c r="J42"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A43" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I43"/>
-      <c r="J43"/>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A44" s="2"/>
-      <c r="I44"/>
-      <c r="J44"/>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A45" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
-      <c r="I45"/>
-      <c r="J45"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A46" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I46"/>
-      <c r="J46"/>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A47" s="2"/>
-      <c r="I47"/>
-      <c r="J47"/>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A48" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C48" s="2"/>
-      <c r="D48" s="2"/>
-      <c r="E48" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I48"/>
-      <c r="J48"/>
-    </row>
+    <row r="38" spans="1:10" ht="6.4" customHeight="1" x14ac:dyDescent="0.5"/>
+    <row r="39" spans="1:10" ht="6.4" customHeight="1" x14ac:dyDescent="0.5"/>
+    <row r="40" spans="1:10" ht="6.4" customHeight="1" x14ac:dyDescent="0.5"/>
+    <row r="41" spans="1:10" ht="6.4" customHeight="1" x14ac:dyDescent="0.5"/>
+    <row r="42" spans="1:10" ht="6.4" customHeight="1" x14ac:dyDescent="0.5"/>
+    <row r="43" spans="1:10" ht="6.4" customHeight="1" x14ac:dyDescent="0.5"/>
+    <row r="44" spans="1:10" ht="6.4" customHeight="1" x14ac:dyDescent="0.5"/>
+    <row r="45" spans="1:10" ht="6.4" customHeight="1" x14ac:dyDescent="0.5"/>
   </sheetData>
   <sheetProtection selectLockedCells="1" sort="0" autoFilter="0" selectUnlockedCells="1"/>
   <protectedRanges>
     <protectedRange sqref="J1" name="Диапазон1"/>
   </protectedRanges>
-  <conditionalFormatting sqref="F12:G12 A11:H11 A9:G10">
+  <conditionalFormatting sqref="A9:G9">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(A9))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="76" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="77" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
beta request tmp implemented, work on port letter tmp in progress
</commit_message>
<xml_diff>
--- a/templates/Request_Contract_Ru.xlsx
+++ b/templates/Request_Contract_Ru.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97F68409-F5FB-4A51-B257-2302FE16DCBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{585A98A1-A305-4466-9AB2-9A8979093110}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-55778" yWindow="-907" windowWidth="28995" windowHeight="15795" xr2:uid="{D30FD3A5-3631-4292-86EF-527B77EA97BF}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{D30FD3A5-3631-4292-86EF-527B77EA97BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Request_Contract" sheetId="1" r:id="rId1"/>
@@ -164,7 +164,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="&quot;1/&quot;#,##0.0&quot; кг&quot;"/>
-    <numFmt numFmtId="172" formatCode="#,##0.00\ &quot;₽&quot;"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;₽&quot;"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -299,7 +299,7 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="172" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -315,17 +315,17 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="172" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf numFmtId="172" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="172" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="172" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="172" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
@@ -726,8 +726,8 @@
   </sheetPr>
   <dimension ref="A1:V45"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="84" zoomScaleNormal="100" zoomScaleSheetLayoutView="84" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A9" zoomScale="84" zoomScaleNormal="100" zoomScaleSheetLayoutView="84" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>

</xml_diff>

<commit_message>
implementing formik in request section
</commit_message>
<xml_diff>
--- a/templates/Request_Contract_Ru.xlsx
+++ b/templates/Request_Contract_Ru.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2DC75E3-F6B7-408A-B955-733E93119299}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C123BA6A-DDEB-40D0-A757-5B295035888E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="27076" windowHeight="16395" xr2:uid="{D30FD3A5-3631-4292-86EF-527B77EA97BF}"/>
+    <workbookView xWindow="-55778" yWindow="-277" windowWidth="28995" windowHeight="15795" xr2:uid="{D30FD3A5-3631-4292-86EF-527B77EA97BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Request_Contract" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Request_Contract!$A$1:$G$45</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Request_Contract!$A$1:$G$46</definedName>
     <definedName name="Банковские_реквизиты">Request_Contract!$A$19</definedName>
-    <definedName name="ВСД">Request_Contract!$A$25</definedName>
-    <definedName name="ВСД_далее">Request_Contract!$A$26</definedName>
+    <definedName name="ВСД">Request_Contract!$A$26</definedName>
+    <definedName name="ВСД_далее">Request_Contract!$A$27</definedName>
     <definedName name="Доставка_условия">Request_Contract!$A$12</definedName>
     <definedName name="Заявка">Request_Contract!$A$4</definedName>
     <definedName name="Заявка_дата">Request_Contract!$G$3</definedName>
@@ -27,7 +27,8 @@
     <definedName name="Заявка_стороны">Request_Contract!$A$6</definedName>
     <definedName name="Оплата_дата">Request_Contract!$A$13</definedName>
     <definedName name="Прибытие">Request_Contract!$A$21</definedName>
-    <definedName name="Приемка">Request_Contract!$A$23</definedName>
+    <definedName name="Приемка1">Request_Contract!$A$23</definedName>
+    <definedName name="Приемка2">Request_Contract!$A$24</definedName>
     <definedName name="Сумма">Request_Contract!$A$11</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -51,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>З А Я В К А</t>
   </si>
@@ -153,6 +154,9 @@
   </si>
   <si>
     <t>Составил заявку:  ________________________________________________________</t>
+  </si>
+  <si>
+    <t>* строка для FCA</t>
   </si>
 </sst>
 </file>
@@ -721,10 +725,10 @@
     <tabColor theme="5" tint="0.39997558519241921"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:V45"/>
+  <dimension ref="A1:V46"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A9" zoomScale="84" zoomScaleNormal="100" zoomScaleSheetLayoutView="84" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A10" zoomScale="84" zoomScaleNormal="100" zoomScaleSheetLayoutView="84" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -1058,33 +1062,35 @@
       <c r="J23"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A24" s="2"/>
+      <c r="A24" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="I24"/>
       <c r="J24"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A25" s="2" t="s">
-        <v>23</v>
-      </c>
+      <c r="A25" s="2"/>
       <c r="I25"/>
       <c r="J25"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A26" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I26"/>
       <c r="J26"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A27" s="2" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="I27"/>
       <c r="J27"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A28" s="2"/>
+      <c r="A28" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="I28"/>
       <c r="J28"/>
     </row>
@@ -1099,60 +1105,64 @@
       <c r="J30"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A31" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="A31" s="2"/>
       <c r="I31"/>
       <c r="J31"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A32" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I32"/>
       <c r="J32"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A33" s="2"/>
+      <c r="A33" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="I33"/>
       <c r="J33"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A34" t="s">
-        <v>32</v>
-      </c>
-      <c r="B34"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
+      <c r="A34" s="2"/>
       <c r="I34"/>
       <c r="J34"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A35" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="A35" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
       <c r="I35"/>
       <c r="J35"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A36" s="2"/>
+      <c r="A36" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="I36"/>
       <c r="J36"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A37" t="s">
-        <v>33</v>
-      </c>
-      <c r="B37"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="21" t="s">
-        <v>13</v>
-      </c>
+      <c r="A37" s="2"/>
       <c r="I37"/>
       <c r="J37"/>
     </row>
-    <row r="38" spans="1:10" ht="6.4" customHeight="1" x14ac:dyDescent="0.5"/>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A38" t="s">
+        <v>33</v>
+      </c>
+      <c r="B38"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="I38"/>
+      <c r="J38"/>
+    </row>
     <row r="39" spans="1:10" ht="6.4" customHeight="1" x14ac:dyDescent="0.5"/>
     <row r="40" spans="1:10" ht="6.4" customHeight="1" x14ac:dyDescent="0.5"/>
     <row r="41" spans="1:10" ht="6.4" customHeight="1" x14ac:dyDescent="0.5"/>
@@ -1160,6 +1170,7 @@
     <row r="43" spans="1:10" ht="6.4" customHeight="1" x14ac:dyDescent="0.5"/>
     <row r="44" spans="1:10" ht="6.4" customHeight="1" x14ac:dyDescent="0.5"/>
     <row r="45" spans="1:10" ht="6.4" customHeight="1" x14ac:dyDescent="0.5"/>
+    <row r="46" spans="1:10" ht="6.4" customHeight="1" x14ac:dyDescent="0.5"/>
   </sheetData>
   <sheetProtection selectLockedCells="1" sort="0" autoFilter="0" selectUnlockedCells="1"/>
   <protectedRanges>

</xml_diff>

<commit_message>
inner market section added to distinct template file request route
</commit_message>
<xml_diff>
--- a/templates/Request_Contract_Ru.xlsx
+++ b/templates/Request_Contract_Ru.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C123BA6A-DDEB-40D0-A757-5B295035888E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C32277FE-5E73-4C1F-9556-BBA5C50D2F37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-55778" yWindow="-277" windowWidth="28995" windowHeight="15795" xr2:uid="{D30FD3A5-3631-4292-86EF-527B77EA97BF}"/>
+    <workbookView xWindow="-57697" yWindow="-277" windowWidth="28995" windowHeight="15795" xr2:uid="{D30FD3A5-3631-4292-86EF-527B77EA97BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Request_Contract" sheetId="1" r:id="rId1"/>
@@ -96,9 +96,6 @@
     <t xml:space="preserve">  _______________________   </t>
   </si>
   <si>
-    <t xml:space="preserve">                                                                                              (Ф.И.О.)                                                                                  (подпись)   </t>
-  </si>
-  <si>
     <t>МФТ "Морской Волк"</t>
   </si>
   <si>
@@ -157,6 +154,9 @@
   </si>
   <si>
     <t>* строка для FCA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                                                              (Ф.И.О.)                                                                                                      (подпись)   </t>
   </si>
 </sst>
 </file>
@@ -377,7 +377,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>1003300</xdr:colOff>
+      <xdr:colOff>1003301</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>7771</xdr:rowOff>
     </xdr:to>
@@ -727,16 +727,16 @@
   </sheetPr>
   <dimension ref="A1:V46"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A10" zoomScale="84" zoomScaleNormal="100" zoomScaleSheetLayoutView="84" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="84" zoomScaleNormal="100" zoomScaleSheetLayoutView="84" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="24.3984375" style="6" customWidth="1"/>
-    <col min="2" max="2" width="21.46484375" style="6" customWidth="1"/>
+    <col min="2" max="2" width="31.796875" style="6" customWidth="1"/>
     <col min="3" max="3" width="7.1328125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="37.6640625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="35.9296875" style="6" customWidth="1"/>
     <col min="5" max="5" width="12.73046875" style="18" customWidth="1"/>
     <col min="6" max="6" width="10.6640625" style="23" customWidth="1"/>
     <col min="7" max="7" width="15.59765625" style="6" customWidth="1"/>
@@ -821,7 +821,7 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.5">
       <c r="A4" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I4"/>
       <c r="J4"/>
@@ -855,7 +855,7 @@
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.5">
       <c r="A6" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I6"/>
       <c r="J6"/>
@@ -887,7 +887,7 @@
       <c r="T7" s="7"/>
       <c r="U7" s="7"/>
     </row>
-    <row r="8" spans="1:22" ht="39" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:22" ht="29.35" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A8" s="3" t="s">
         <v>2</v>
       </c>
@@ -901,10 +901,10 @@
         <v>5</v>
       </c>
       <c r="E8" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="24" t="s">
         <v>30</v>
-      </c>
-      <c r="F8" s="24" t="s">
-        <v>31</v>
       </c>
       <c r="G8" s="25" t="s">
         <v>6</v>
@@ -925,16 +925,16 @@
     </row>
     <row r="9" spans="1:22" ht="68.650000000000006" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="C9" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="11" t="s">
-        <v>17</v>
-      </c>
       <c r="D9" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E9" s="20">
         <v>172939</v>
@@ -966,7 +966,7 @@
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.5">
       <c r="A11" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G11" s="23"/>
       <c r="I11"/>
@@ -974,7 +974,7 @@
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.5">
       <c r="A12" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G12" s="23"/>
       <c r="I12"/>
@@ -982,7 +982,7 @@
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.5">
       <c r="A13" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G13" s="23"/>
       <c r="I13"/>
@@ -1014,7 +1014,7 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A17" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G17" s="23"/>
       <c r="I17"/>
@@ -1028,7 +1028,7 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A19" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G19" s="23"/>
       <c r="I19"/>
@@ -1042,7 +1042,7 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A21" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G21" s="23"/>
       <c r="I21"/>
@@ -1056,14 +1056,14 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A23" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I23"/>
       <c r="J23"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A24" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I24"/>
       <c r="J24"/>
@@ -1075,14 +1075,14 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A26" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I26"/>
       <c r="J26"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A27" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I27"/>
       <c r="J27"/>
@@ -1130,7 +1130,7 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A35" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B35"/>
       <c r="C35" s="2"/>
@@ -1140,7 +1140,7 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A36" s="2" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="I36"/>
       <c r="J36"/>
@@ -1152,7 +1152,7 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A38" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B38"/>
       <c r="C38" s="2"/>
@@ -1182,7 +1182,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="77" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="73" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
invoice only feature in request section added + some styles fixed
</commit_message>
<xml_diff>
--- a/templates/Request_Contract_Ru.xlsx
+++ b/templates/Request_Contract_Ru.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C32277FE-5E73-4C1F-9556-BBA5C50D2F37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0187DA21-4923-4C04-997E-84D6284A30A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57697" yWindow="-277" windowWidth="28995" windowHeight="15795" xr2:uid="{D30FD3A5-3631-4292-86EF-527B77EA97BF}"/>
+    <workbookView xWindow="-54848" yWindow="-277" windowWidth="28065" windowHeight="16394" xr2:uid="{D30FD3A5-3631-4292-86EF-527B77EA97BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Request_Contract" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <definedName name="Банковские_реквизиты">Request_Contract!$A$19</definedName>
     <definedName name="ВСД">Request_Contract!$A$26</definedName>
     <definedName name="ВСД_далее">Request_Contract!$A$27</definedName>
+    <definedName name="ВСЭ">Request_Contract!$A$28</definedName>
     <definedName name="Доставка_условия">Request_Contract!$A$12</definedName>
     <definedName name="Заявка">Request_Contract!$A$4</definedName>
     <definedName name="Заявка_дата">Request_Contract!$G$3</definedName>
@@ -727,8 +728,8 @@
   </sheetPr>
   <dimension ref="A1:V46"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="84" zoomScaleNormal="100" zoomScaleSheetLayoutView="84" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A8" zoomScale="84" zoomScaleNormal="100" zoomScaleSheetLayoutView="84" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>

</xml_diff>

<commit_message>
rows beta counting values feature in excel tmps added (string type replaced with count + cell are formatting with Excel formats)
</commit_message>
<xml_diff>
--- a/templates/Request_Contract_Ru.xlsx
+++ b/templates/Request_Contract_Ru.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0187DA21-4923-4C04-997E-84D6284A30A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20EB8B6F-42F8-4C2E-8DEA-378B268CD639}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-54848" yWindow="-277" windowWidth="28065" windowHeight="16394" xr2:uid="{D30FD3A5-3631-4292-86EF-527B77EA97BF}"/>
+    <workbookView xWindow="-55778" yWindow="-277" windowWidth="28995" windowHeight="16394" xr2:uid="{D30FD3A5-3631-4292-86EF-527B77EA97BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Request_Contract" sheetId="1" r:id="rId1"/>
@@ -301,9 +301,6 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
@@ -327,7 +324,10 @@
     <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
@@ -728,8 +728,8 @@
   </sheetPr>
   <dimension ref="A1:V46"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A8" zoomScale="84" zoomScaleNormal="100" zoomScaleSheetLayoutView="84" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A2" zoomScale="84" zoomScaleNormal="100" zoomScaleSheetLayoutView="84" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -738,8 +738,8 @@
     <col min="2" max="2" width="31.796875" style="6" customWidth="1"/>
     <col min="3" max="3" width="7.1328125" style="6" customWidth="1"/>
     <col min="4" max="4" width="35.9296875" style="6" customWidth="1"/>
-    <col min="5" max="5" width="12.73046875" style="18" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" style="23" customWidth="1"/>
+    <col min="5" max="5" width="12.73046875" style="17" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" style="22" customWidth="1"/>
     <col min="7" max="7" width="15.59765625" style="6" customWidth="1"/>
     <col min="8" max="8" width="14.33203125" style="6" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.796875" style="6"/>
@@ -764,8 +764,8 @@
       <c r="B1" s="14"/>
       <c r="C1" s="14"/>
       <c r="D1" s="14"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="22"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="21"/>
       <c r="G1" s="14"/>
       <c r="H1" s="13"/>
       <c r="I1"/>
@@ -901,13 +901,13 @@
       <c r="D8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="19" t="s">
+      <c r="E8" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="24" t="s">
+      <c r="F8" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="G8" s="25" t="s">
+      <c r="G8" s="24" t="s">
         <v>6</v>
       </c>
       <c r="H8"/>
@@ -937,10 +937,10 @@
       <c r="D9" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="20">
+      <c r="E9" s="19">
         <v>172939</v>
       </c>
-      <c r="F9" s="16">
+      <c r="F9" s="25">
         <v>36</v>
       </c>
       <c r="G9" s="26">
@@ -961,7 +961,7 @@
       <c r="T9" s="7"/>
     </row>
     <row r="10" spans="1:22" ht="79.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="G10" s="23"/>
+      <c r="G10" s="22"/>
       <c r="I10"/>
       <c r="J10"/>
     </row>
@@ -969,7 +969,7 @@
       <c r="A11" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="G11" s="23"/>
+      <c r="G11" s="22"/>
       <c r="I11"/>
       <c r="J11"/>
     </row>
@@ -977,7 +977,7 @@
       <c r="A12" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G12" s="23"/>
+      <c r="G12" s="22"/>
       <c r="I12"/>
       <c r="J12"/>
     </row>
@@ -985,7 +985,7 @@
       <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G13" s="23"/>
+      <c r="G13" s="22"/>
       <c r="I13"/>
       <c r="J13"/>
     </row>
@@ -993,7 +993,7 @@
       <c r="A14" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G14" s="23"/>
+      <c r="G14" s="22"/>
       <c r="I14"/>
       <c r="J14"/>
     </row>
@@ -1001,7 +1001,7 @@
       <c r="A15" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G15" s="23"/>
+      <c r="G15" s="22"/>
       <c r="I15"/>
       <c r="J15"/>
     </row>
@@ -1009,7 +1009,7 @@
       <c r="A16" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G16" s="23"/>
+      <c r="G16" s="22"/>
       <c r="I16"/>
       <c r="J16"/>
     </row>
@@ -1017,13 +1017,13 @@
       <c r="A17" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="G17" s="23"/>
+      <c r="G17" s="22"/>
       <c r="I17"/>
       <c r="J17"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A18" s="2"/>
-      <c r="G18" s="23"/>
+      <c r="G18" s="22"/>
       <c r="I18"/>
       <c r="J18"/>
     </row>
@@ -1031,13 +1031,13 @@
       <c r="A19" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G19" s="23"/>
+      <c r="G19" s="22"/>
       <c r="I19"/>
       <c r="J19"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A20" s="2"/>
-      <c r="G20" s="23"/>
+      <c r="G20" s="22"/>
       <c r="I20"/>
       <c r="J20"/>
     </row>
@@ -1045,13 +1045,13 @@
       <c r="A21" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G21" s="23"/>
+      <c r="G21" s="22"/>
       <c r="I21"/>
       <c r="J21"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A22" s="2"/>
-      <c r="G22" s="23"/>
+      <c r="G22" s="22"/>
       <c r="I22"/>
       <c r="J22"/>
     </row>
@@ -1158,7 +1158,7 @@
       <c r="B38"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
-      <c r="E38" s="21" t="s">
+      <c r="E38" s="20" t="s">
         <v>13</v>
       </c>
       <c r="I38"/>

</xml_diff>

<commit_message>
format export invoice price fixed
</commit_message>
<xml_diff>
--- a/templates/Request_Contract_Ru.xlsx
+++ b/templates/Request_Contract_Ru.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20EB8B6F-42F8-4C2E-8DEA-378B268CD639}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{898CE546-1065-4BA8-AE66-74E9442DF833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-55778" yWindow="-277" windowWidth="28995" windowHeight="16394" xr2:uid="{D30FD3A5-3631-4292-86EF-527B77EA97BF}"/>
+    <workbookView xWindow="28702" yWindow="83" windowWidth="27076" windowHeight="16995" xr2:uid="{D30FD3A5-3631-4292-86EF-527B77EA97BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Request_Contract" sheetId="1" r:id="rId1"/>
@@ -262,7 +262,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -323,12 +323,6 @@
     </xf>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -426,9 +420,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -466,7 +460,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -572,7 +566,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -714,7 +708,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -728,8 +722,8 @@
   </sheetPr>
   <dimension ref="A1:V46"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A2" zoomScale="84" zoomScaleNormal="100" zoomScaleSheetLayoutView="84" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A3" zoomScale="84" zoomScaleNormal="100" zoomScaleSheetLayoutView="84" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -940,10 +934,10 @@
       <c r="E9" s="19">
         <v>172939</v>
       </c>
-      <c r="F9" s="25">
+      <c r="F9" s="11">
         <v>36</v>
       </c>
-      <c r="G9" s="26">
+      <c r="G9" s="1">
         <v>6225804</v>
       </c>
       <c r="H9"/>

</xml_diff>

<commit_message>
working on invoicesOnly Inner Tmp
</commit_message>
<xml_diff>
--- a/templates/Request_Contract_Ru.xlsx
+++ b/templates/Request_Contract_Ru.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{898CE546-1065-4BA8-AE66-74E9442DF833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99AB195F-47CB-49F0-AEA1-6A9A73DDAA0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28702" yWindow="83" windowWidth="27076" windowHeight="16995" xr2:uid="{D30FD3A5-3631-4292-86EF-527B77EA97BF}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="27076" windowHeight="16395" xr2:uid="{D30FD3A5-3631-4292-86EF-527B77EA97BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Request_Contract" sheetId="1" r:id="rId1"/>
@@ -164,11 +164,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
+    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;₽&quot;_-;\-* #,##0.00\ &quot;₽&quot;_-;_-* &quot;-&quot;??\ &quot;₽&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="&quot;1/&quot;#,##0.0&quot; кг&quot;"/>
     <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;₽&quot;"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -219,6 +220,14 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -258,11 +267,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -309,9 +319,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -324,8 +331,18 @@
     <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Обычный 2" xfId="1" xr:uid="{FCCBD63C-76D8-458A-A4D4-01A44EBCF99F}"/>
   </cellStyles>
@@ -722,8 +739,8 @@
   </sheetPr>
   <dimension ref="A1:V46"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A3" zoomScale="84" zoomScaleNormal="100" zoomScaleSheetLayoutView="84" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="84" zoomScaleNormal="100" zoomScaleSheetLayoutView="84" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -733,7 +750,7 @@
     <col min="3" max="3" width="7.1328125" style="6" customWidth="1"/>
     <col min="4" max="4" width="35.9296875" style="6" customWidth="1"/>
     <col min="5" max="5" width="12.73046875" style="17" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" style="22" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" style="21" customWidth="1"/>
     <col min="7" max="7" width="15.59765625" style="6" customWidth="1"/>
     <col min="8" max="8" width="14.33203125" style="6" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.796875" style="6"/>
@@ -759,7 +776,7 @@
       <c r="C1" s="14"/>
       <c r="D1" s="14"/>
       <c r="E1" s="16"/>
-      <c r="F1" s="21"/>
+      <c r="F1" s="20"/>
       <c r="G1" s="14"/>
       <c r="H1" s="13"/>
       <c r="I1"/>
@@ -898,10 +915,10 @@
       <c r="E8" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="23" t="s">
+      <c r="F8" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="G8" s="24" t="s">
+      <c r="G8" s="23" t="s">
         <v>6</v>
       </c>
       <c r="H8"/>
@@ -918,7 +935,7 @@
       <c r="S8" s="7"/>
       <c r="T8" s="7"/>
     </row>
-    <row r="9" spans="1:22" ht="68.650000000000006" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:22" ht="52.9" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A9" s="4" t="s">
         <v>14</v>
       </c>
@@ -931,13 +948,13 @@
       <c r="D9" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="19">
+      <c r="E9" s="26">
         <v>172939</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="25">
         <v>36</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G9" s="24">
         <v>6225804</v>
       </c>
       <c r="H9"/>
@@ -955,7 +972,7 @@
       <c r="T9" s="7"/>
     </row>
     <row r="10" spans="1:22" ht="79.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="G10" s="22"/>
+      <c r="G10" s="21"/>
       <c r="I10"/>
       <c r="J10"/>
     </row>
@@ -963,7 +980,7 @@
       <c r="A11" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="G11" s="22"/>
+      <c r="G11" s="21"/>
       <c r="I11"/>
       <c r="J11"/>
     </row>
@@ -971,7 +988,7 @@
       <c r="A12" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G12" s="22"/>
+      <c r="G12" s="21"/>
       <c r="I12"/>
       <c r="J12"/>
     </row>
@@ -979,7 +996,7 @@
       <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G13" s="22"/>
+      <c r="G13" s="21"/>
       <c r="I13"/>
       <c r="J13"/>
     </row>
@@ -987,7 +1004,7 @@
       <c r="A14" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G14" s="22"/>
+      <c r="G14" s="21"/>
       <c r="I14"/>
       <c r="J14"/>
     </row>
@@ -995,7 +1012,7 @@
       <c r="A15" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G15" s="22"/>
+      <c r="G15" s="21"/>
       <c r="I15"/>
       <c r="J15"/>
     </row>
@@ -1003,7 +1020,7 @@
       <c r="A16" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G16" s="22"/>
+      <c r="G16" s="21"/>
       <c r="I16"/>
       <c r="J16"/>
     </row>
@@ -1011,13 +1028,13 @@
       <c r="A17" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="G17" s="22"/>
+      <c r="G17" s="21"/>
       <c r="I17"/>
       <c r="J17"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A18" s="2"/>
-      <c r="G18" s="22"/>
+      <c r="G18" s="21"/>
       <c r="I18"/>
       <c r="J18"/>
     </row>
@@ -1025,13 +1042,13 @@
       <c r="A19" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G19" s="22"/>
+      <c r="G19" s="21"/>
       <c r="I19"/>
       <c r="J19"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A20" s="2"/>
-      <c r="G20" s="22"/>
+      <c r="G20" s="21"/>
       <c r="I20"/>
       <c r="J20"/>
     </row>
@@ -1039,13 +1056,13 @@
       <c r="A21" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G21" s="22"/>
+      <c r="G21" s="21"/>
       <c r="I21"/>
       <c r="J21"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A22" s="2"/>
-      <c r="G22" s="22"/>
+      <c r="G22" s="21"/>
       <c r="I22"/>
       <c r="J22"/>
     </row>
@@ -1152,7 +1169,7 @@
       <c r="B38"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
-      <c r="E38" s="20" t="s">
+      <c r="E38" s="19" t="s">
         <v>13</v>
       </c>
       <c r="I38"/>

</xml_diff>